<commit_message>
Changes in charging stations
</commit_message>
<xml_diff>
--- a/CHARGER STATIONS/Electromaps.xlsx
+++ b/CHARGER STATIONS/Electromaps.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Downloads\9no Semestre\Estancias\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://correoipn-my.sharepoint.com/personal/eamadorm1501_alumno_ipn_mx/Documents/GITHUB/charger-stations-data-cleaned/CHARGER STATIONS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA4BE88B-DD0D-473B-9F8B-1027797788FE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{AA4BE88B-DD0D-473B-9F8B-1027797788FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F46719D5-E4E5-45F6-AB44-E8AF99885B24}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{178D4FA0-2D65-4D1B-875E-35891CE86E72}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{178D4FA0-2D65-4D1B-875E-35891CE86E72}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -797,7 +797,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -811,8 +811,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -846,6 +852,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -903,7 +915,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -932,14 +944,25 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1255,10 +1278,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B577CC59-3E9C-435B-9F39-7E1713DD7AD3}">
-  <dimension ref="A1:V83"/>
+  <dimension ref="A1:W83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="R88" sqref="R88"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B40" sqref="A40:XFD40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1270,23 +1293,23 @@
     <col min="5" max="5" width="42" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="37.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17" style="1" customWidth="1"/>
-    <col min="9" max="9" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="8.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="26.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="21.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="20.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="11.42578125" style="1"/>
-    <col min="17" max="17" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="20" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="19.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="21" width="11.42578125" style="1"/>
-    <col min="22" max="22" width="23.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="16384" width="11.42578125" style="1"/>
+    <col min="12" max="12" width="17" style="1" customWidth="1"/>
+    <col min="13" max="13" width="21.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="20.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="11.42578125" style="1"/>
+    <col min="18" max="18" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="20" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="19.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="11.42578125" style="1"/>
+    <col min="23" max="23" width="23.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1309,52 +1332,52 @@
         <v>4</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="K1" s="2" t="s">
-        <v>6</v>
-      </c>
       <c r="L1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="M1" s="2" t="s">
         <v>244</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>198</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>245</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="R1" s="3" t="s">
         <v>246</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="S1" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="T1" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="U1" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="U1" s="3" t="s">
+      <c r="V1" s="3" t="s">
         <v>247</v>
       </c>
-      <c r="V1" s="3" t="s">
+      <c r="W1" s="3" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1377,24 +1400,23 @@
         <v>12</v>
       </c>
       <c r="H2" s="2">
-        <v>1</v>
-      </c>
-      <c r="I2" s="2">
         <v>3.7</v>
       </c>
+      <c r="I2" s="2" t="s">
+        <v>9</v>
+      </c>
       <c r="J2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="K2" s="2" t="s">
-        <v>9</v>
-      </c>
       <c r="L2" s="2">
         <v>1</v>
       </c>
       <c r="M2" s="2">
         <v>1</v>
       </c>
-      <c r="N2" s="2"/>
+      <c r="N2" s="2">
+        <v>1</v>
+      </c>
       <c r="O2" s="2"/>
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
@@ -1403,8 +1425,9 @@
       <c r="T2" s="2"/>
       <c r="U2" s="2"/>
       <c r="V2" s="2"/>
-    </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W2" s="2"/>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -1427,22 +1450,21 @@
         <v>12</v>
       </c>
       <c r="H3" s="2">
-        <v>2</v>
-      </c>
-      <c r="I3" s="2">
         <v>3.7</v>
       </c>
+      <c r="I3" s="2"/>
       <c r="J3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="K3" s="2"/>
       <c r="L3" s="2">
         <v>2</v>
       </c>
       <c r="M3" s="2">
         <v>2</v>
       </c>
-      <c r="N3" s="2"/>
+      <c r="N3" s="2">
+        <v>2</v>
+      </c>
       <c r="O3" s="2"/>
       <c r="P3" s="2"/>
       <c r="Q3" s="2"/>
@@ -1451,8 +1473,9 @@
       <c r="T3" s="2"/>
       <c r="U3" s="2"/>
       <c r="V3" s="2"/>
-    </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W3" s="2"/>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -1475,22 +1498,21 @@
         <v>12</v>
       </c>
       <c r="H4" s="2">
-        <v>2</v>
-      </c>
-      <c r="I4" s="2">
         <v>3.7</v>
       </c>
+      <c r="I4" s="2"/>
       <c r="J4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="K4" s="2"/>
       <c r="L4" s="2">
         <v>2</v>
       </c>
       <c r="M4" s="2">
         <v>2</v>
       </c>
-      <c r="N4" s="2"/>
+      <c r="N4" s="2">
+        <v>2</v>
+      </c>
       <c r="O4" s="2"/>
       <c r="P4" s="2"/>
       <c r="Q4" s="2"/>
@@ -1499,8 +1521,9 @@
       <c r="T4" s="2"/>
       <c r="U4" s="2"/>
       <c r="V4" s="2"/>
-    </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W4" s="2"/>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -1523,24 +1546,23 @@
         <v>12</v>
       </c>
       <c r="H5" s="2">
-        <v>1</v>
-      </c>
-      <c r="I5" s="2">
         <v>6.6</v>
       </c>
+      <c r="I5" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="J5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="K5" s="2" t="s">
-        <v>25</v>
-      </c>
       <c r="L5" s="2">
         <v>1</v>
       </c>
       <c r="M5" s="2">
         <v>1</v>
       </c>
-      <c r="N5" s="2"/>
+      <c r="N5" s="2">
+        <v>1</v>
+      </c>
       <c r="O5" s="2"/>
       <c r="P5" s="2"/>
       <c r="Q5" s="2"/>
@@ -1549,8 +1571,9 @@
       <c r="T5" s="2"/>
       <c r="U5" s="2"/>
       <c r="V5" s="2"/>
-    </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W5" s="2"/>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -1573,24 +1596,23 @@
         <v>12</v>
       </c>
       <c r="H6" s="2">
-        <v>1</v>
-      </c>
-      <c r="I6" s="2">
         <v>6</v>
       </c>
+      <c r="I6" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="J6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="K6" s="2" t="s">
-        <v>28</v>
-      </c>
       <c r="L6" s="2">
         <v>1</v>
       </c>
       <c r="M6" s="2">
         <v>1</v>
       </c>
-      <c r="N6" s="2"/>
+      <c r="N6" s="2">
+        <v>1</v>
+      </c>
       <c r="O6" s="2"/>
       <c r="P6" s="2"/>
       <c r="Q6" s="2"/>
@@ -1599,8 +1621,9 @@
       <c r="T6" s="2"/>
       <c r="U6" s="2"/>
       <c r="V6" s="2"/>
-    </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W6" s="2"/>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -1623,24 +1646,23 @@
         <v>12</v>
       </c>
       <c r="H7" s="2">
-        <v>1</v>
-      </c>
-      <c r="I7" s="2">
         <v>6.6</v>
       </c>
+      <c r="I7" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="J7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="K7" s="2" t="s">
-        <v>25</v>
-      </c>
       <c r="L7" s="2">
         <v>1</v>
       </c>
       <c r="M7" s="2">
         <v>1</v>
       </c>
-      <c r="N7" s="2"/>
+      <c r="N7" s="2">
+        <v>1</v>
+      </c>
       <c r="O7" s="2"/>
       <c r="P7" s="2"/>
       <c r="Q7" s="2"/>
@@ -1649,8 +1671,9 @@
       <c r="T7" s="2"/>
       <c r="U7" s="2"/>
       <c r="V7" s="2"/>
-    </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W7" s="2"/>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -1671,36 +1694,36 @@
         <v>34</v>
       </c>
       <c r="H8" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="L8" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="I8" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="J8" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="K8" s="2"/>
-      <c r="L8" s="2">
+      <c r="M8" s="2">
         <v>3</v>
       </c>
-      <c r="M8" s="2">
-        <v>1</v>
-      </c>
-      <c r="N8" s="2"/>
+      <c r="N8" s="2">
+        <v>1</v>
+      </c>
       <c r="O8" s="2"/>
-      <c r="P8" s="2">
-        <v>1</v>
-      </c>
-      <c r="Q8" s="2"/>
+      <c r="P8" s="2"/>
+      <c r="Q8" s="2">
+        <v>1</v>
+      </c>
       <c r="R8" s="2"/>
       <c r="S8" s="2"/>
       <c r="T8" s="2"/>
-      <c r="U8" s="2">
-        <v>1</v>
-      </c>
-      <c r="V8" s="2"/>
-    </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="U8" s="2"/>
+      <c r="V8" s="2">
+        <v>1</v>
+      </c>
+      <c r="W8" s="2"/>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -1723,22 +1746,21 @@
         <v>12</v>
       </c>
       <c r="H9" s="2">
-        <v>1</v>
-      </c>
-      <c r="I9" s="2">
         <v>6</v>
       </c>
+      <c r="I9" s="2"/>
       <c r="J9" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="K9" s="2"/>
       <c r="L9" s="2">
         <v>1</v>
       </c>
       <c r="M9" s="2">
         <v>1</v>
       </c>
-      <c r="N9" s="2"/>
+      <c r="N9" s="2">
+        <v>1</v>
+      </c>
       <c r="O9" s="2"/>
       <c r="P9" s="2"/>
       <c r="Q9" s="2"/>
@@ -1747,8 +1769,9 @@
       <c r="T9" s="2"/>
       <c r="U9" s="2"/>
       <c r="V9" s="2"/>
-    </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W9" s="2"/>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -1771,32 +1794,32 @@
         <v>42</v>
       </c>
       <c r="H10" s="2">
-        <v>1</v>
-      </c>
-      <c r="I10" s="2">
         <v>3.7</v>
       </c>
+      <c r="I10" s="2"/>
       <c r="J10" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="K10" s="2"/>
       <c r="L10" s="2">
         <v>1</v>
       </c>
-      <c r="M10" s="2"/>
+      <c r="M10" s="2">
+        <v>1</v>
+      </c>
       <c r="N10" s="2"/>
       <c r="O10" s="2"/>
-      <c r="P10" s="2">
-        <v>1</v>
-      </c>
-      <c r="Q10" s="2"/>
+      <c r="P10" s="2"/>
+      <c r="Q10" s="2">
+        <v>1</v>
+      </c>
       <c r="R10" s="2"/>
       <c r="S10" s="2"/>
       <c r="T10" s="2"/>
       <c r="U10" s="2"/>
       <c r="V10" s="2"/>
-    </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W10" s="2"/>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -1819,34 +1842,34 @@
         <v>45</v>
       </c>
       <c r="H11" s="2">
-        <v>1</v>
-      </c>
-      <c r="I11" s="2">
         <v>50</v>
       </c>
+      <c r="I11" s="2" t="s">
+        <v>46</v>
+      </c>
       <c r="J11" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="K11" s="2" t="s">
-        <v>46</v>
-      </c>
       <c r="L11" s="2">
         <v>1</v>
       </c>
-      <c r="M11" s="2"/>
+      <c r="M11" s="2">
+        <v>1</v>
+      </c>
       <c r="N11" s="2"/>
       <c r="O11" s="2"/>
       <c r="P11" s="2"/>
       <c r="Q11" s="2"/>
       <c r="R11" s="2"/>
       <c r="S11" s="2"/>
-      <c r="T11" s="2">
-        <v>1</v>
-      </c>
-      <c r="U11" s="2"/>
+      <c r="T11" s="2"/>
+      <c r="U11" s="2">
+        <v>1</v>
+      </c>
       <c r="V11" s="2"/>
-    </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W11" s="2"/>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -1869,24 +1892,23 @@
         <v>12</v>
       </c>
       <c r="H12" s="2">
-        <v>1</v>
-      </c>
-      <c r="I12" s="2">
         <v>6</v>
       </c>
+      <c r="I12" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="J12" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="K12" s="2" t="s">
-        <v>25</v>
-      </c>
       <c r="L12" s="2">
         <v>1</v>
       </c>
       <c r="M12" s="2">
         <v>1</v>
       </c>
-      <c r="N12" s="2"/>
+      <c r="N12" s="2">
+        <v>1</v>
+      </c>
       <c r="O12" s="2"/>
       <c r="P12" s="2"/>
       <c r="Q12" s="2"/>
@@ -1895,8 +1917,9 @@
       <c r="T12" s="2"/>
       <c r="U12" s="2"/>
       <c r="V12" s="2"/>
-    </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W12" s="2"/>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -1919,24 +1942,23 @@
         <v>12</v>
       </c>
       <c r="H13" s="2">
-        <v>1</v>
-      </c>
-      <c r="I13" s="2">
         <v>7.4</v>
       </c>
+      <c r="I13" s="2" t="s">
+        <v>9</v>
+      </c>
       <c r="J13" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="K13" s="2" t="s">
-        <v>9</v>
-      </c>
       <c r="L13" s="2">
         <v>1</v>
       </c>
       <c r="M13" s="2">
         <v>1</v>
       </c>
-      <c r="N13" s="2"/>
+      <c r="N13" s="2">
+        <v>1</v>
+      </c>
       <c r="O13" s="2"/>
       <c r="P13" s="2"/>
       <c r="Q13" s="2"/>
@@ -1945,8 +1967,9 @@
       <c r="T13" s="2"/>
       <c r="U13" s="2"/>
       <c r="V13" s="2"/>
-    </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W13" s="2"/>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -1969,34 +1992,34 @@
         <v>55</v>
       </c>
       <c r="H14" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="L14" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="I14" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="J14" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="K14" s="2"/>
-      <c r="L14" s="2">
+      <c r="M14" s="2">
         <v>4</v>
       </c>
-      <c r="M14" s="2">
-        <v>1</v>
-      </c>
-      <c r="N14" s="2"/>
+      <c r="N14" s="2">
+        <v>1</v>
+      </c>
       <c r="O14" s="2"/>
       <c r="P14" s="2"/>
       <c r="Q14" s="2"/>
       <c r="R14" s="2"/>
-      <c r="S14" s="2">
+      <c r="S14" s="2"/>
+      <c r="T14" s="2">
         <v>3</v>
       </c>
-      <c r="T14" s="2"/>
       <c r="U14" s="2"/>
       <c r="V14" s="2"/>
-    </row>
-    <row r="15" spans="1:22" ht="30" x14ac:dyDescent="0.25">
+      <c r="W14" s="2"/>
+    </row>
+    <row r="15" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -2019,24 +2042,23 @@
         <v>61</v>
       </c>
       <c r="H15" s="2">
-        <v>1</v>
-      </c>
-      <c r="I15" s="2">
         <v>3.7</v>
       </c>
+      <c r="I15" s="2" t="s">
+        <v>77</v>
+      </c>
       <c r="J15" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="K15" s="2" t="s">
-        <v>77</v>
-      </c>
       <c r="L15" s="2">
         <v>1</v>
       </c>
       <c r="M15" s="2">
         <v>1</v>
       </c>
-      <c r="N15" s="2"/>
+      <c r="N15" s="2">
+        <v>1</v>
+      </c>
       <c r="O15" s="2"/>
       <c r="P15" s="2"/>
       <c r="Q15" s="2"/>
@@ -2045,8 +2067,9 @@
       <c r="T15" s="2"/>
       <c r="U15" s="2"/>
       <c r="V15" s="2"/>
-    </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W15" s="2"/>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -2069,32 +2092,32 @@
         <v>65</v>
       </c>
       <c r="H16" s="2">
-        <v>2</v>
-      </c>
-      <c r="I16" s="2">
         <v>14</v>
       </c>
+      <c r="I16" s="2"/>
       <c r="J16" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="K16" s="2"/>
       <c r="L16" s="2">
         <v>2</v>
       </c>
-      <c r="M16" s="2"/>
+      <c r="M16" s="2">
+        <v>2</v>
+      </c>
       <c r="N16" s="2"/>
       <c r="O16" s="2"/>
       <c r="P16" s="2"/>
       <c r="Q16" s="2"/>
       <c r="R16" s="2"/>
-      <c r="S16" s="2">
-        <v>2</v>
-      </c>
-      <c r="T16" s="2"/>
+      <c r="S16" s="2"/>
+      <c r="T16" s="2">
+        <v>2</v>
+      </c>
       <c r="U16" s="2"/>
       <c r="V16" s="2"/>
-    </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W16" s="2"/>
+    </row>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -2117,22 +2140,21 @@
         <v>12</v>
       </c>
       <c r="H17" s="2">
-        <v>1</v>
-      </c>
-      <c r="I17" s="2">
         <v>6</v>
       </c>
+      <c r="I17" s="2"/>
       <c r="J17" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="K17" s="2"/>
       <c r="L17" s="2">
         <v>1</v>
       </c>
       <c r="M17" s="2">
         <v>1</v>
       </c>
-      <c r="N17" s="2"/>
+      <c r="N17" s="2">
+        <v>1</v>
+      </c>
       <c r="O17" s="2"/>
       <c r="P17" s="2"/>
       <c r="Q17" s="2"/>
@@ -2141,8 +2163,9 @@
       <c r="T17" s="2"/>
       <c r="U17" s="2"/>
       <c r="V17" s="2"/>
-    </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W17" s="2"/>
+    </row>
+    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -2165,36 +2188,36 @@
         <v>73</v>
       </c>
       <c r="H18" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="L18" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="I18" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="J18" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="K18" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="L18" s="2">
-        <v>2</v>
-      </c>
-      <c r="M18" s="2"/>
+      <c r="M18" s="2">
+        <v>2</v>
+      </c>
       <c r="N18" s="2"/>
-      <c r="O18" s="2">
-        <v>1</v>
-      </c>
-      <c r="P18" s="2"/>
+      <c r="O18" s="2"/>
+      <c r="P18" s="2">
+        <v>1</v>
+      </c>
       <c r="Q18" s="2"/>
       <c r="R18" s="2"/>
       <c r="S18" s="2"/>
       <c r="T18" s="2"/>
-      <c r="U18" s="2">
-        <v>1</v>
-      </c>
-      <c r="V18" s="2"/>
-    </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="U18" s="2"/>
+      <c r="V18" s="2">
+        <v>1</v>
+      </c>
+      <c r="W18" s="2"/>
+    </row>
+    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -2217,21 +2240,20 @@
         <v>81</v>
       </c>
       <c r="H19" s="2">
-        <v>1</v>
-      </c>
-      <c r="I19" s="2">
         <v>7.4</v>
       </c>
+      <c r="I19" s="2" t="s">
+        <v>82</v>
+      </c>
       <c r="J19" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="K19" s="2" t="s">
-        <v>82</v>
-      </c>
       <c r="L19" s="2">
         <v>1</v>
       </c>
-      <c r="M19" s="2"/>
+      <c r="M19" s="2">
+        <v>1</v>
+      </c>
       <c r="N19" s="2"/>
       <c r="O19" s="2"/>
       <c r="P19" s="2"/>
@@ -2240,11 +2262,12 @@
       <c r="S19" s="2"/>
       <c r="T19" s="2"/>
       <c r="U19" s="2"/>
-      <c r="V19" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="V19" s="2"/>
+      <c r="W19" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -2267,24 +2290,23 @@
         <v>12</v>
       </c>
       <c r="H20" s="2">
-        <v>1</v>
-      </c>
-      <c r="I20" s="2">
         <v>6</v>
       </c>
+      <c r="I20" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="J20" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="K20" s="2" t="s">
-        <v>25</v>
-      </c>
       <c r="L20" s="2">
         <v>1</v>
       </c>
       <c r="M20" s="2">
         <v>1</v>
       </c>
-      <c r="N20" s="2"/>
+      <c r="N20" s="2">
+        <v>1</v>
+      </c>
       <c r="O20" s="2"/>
       <c r="P20" s="2"/>
       <c r="Q20" s="2"/>
@@ -2293,8 +2315,9 @@
       <c r="T20" s="2"/>
       <c r="U20" s="2"/>
       <c r="V20" s="2"/>
-    </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W20" s="2"/>
+    </row>
+    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>20</v>
       </c>
@@ -2317,22 +2340,21 @@
         <v>12</v>
       </c>
       <c r="H21" s="2">
-        <v>1</v>
-      </c>
-      <c r="I21" s="2">
         <v>6</v>
       </c>
+      <c r="I21" s="2"/>
       <c r="J21" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="K21" s="2"/>
       <c r="L21" s="2">
         <v>1</v>
       </c>
       <c r="M21" s="2">
         <v>1</v>
       </c>
-      <c r="N21" s="2"/>
+      <c r="N21" s="2">
+        <v>1</v>
+      </c>
       <c r="O21" s="2"/>
       <c r="P21" s="2"/>
       <c r="Q21" s="2"/>
@@ -2341,8 +2363,9 @@
       <c r="T21" s="2"/>
       <c r="U21" s="2"/>
       <c r="V21" s="2"/>
-    </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W21" s="2"/>
+    </row>
+    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>21</v>
       </c>
@@ -2365,34 +2388,34 @@
         <v>42</v>
       </c>
       <c r="H22" s="2">
-        <v>1</v>
-      </c>
-      <c r="I22" s="2">
         <v>3.7</v>
       </c>
+      <c r="I22" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="J22" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="K22" s="2" t="s">
-        <v>25</v>
-      </c>
       <c r="L22" s="2">
         <v>1</v>
       </c>
-      <c r="M22" s="2"/>
+      <c r="M22" s="2">
+        <v>1</v>
+      </c>
       <c r="N22" s="2"/>
       <c r="O22" s="2"/>
-      <c r="P22" s="2">
-        <v>1</v>
-      </c>
-      <c r="Q22" s="2"/>
+      <c r="P22" s="2"/>
+      <c r="Q22" s="2">
+        <v>1</v>
+      </c>
       <c r="R22" s="2"/>
       <c r="S22" s="2"/>
       <c r="T22" s="2"/>
       <c r="U22" s="2"/>
       <c r="V22" s="2"/>
-    </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W22" s="2"/>
+    </row>
+    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>22</v>
       </c>
@@ -2415,24 +2438,23 @@
         <v>12</v>
       </c>
       <c r="H23" s="2">
-        <v>1</v>
-      </c>
-      <c r="I23" s="2">
         <v>6.6</v>
       </c>
+      <c r="I23" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="J23" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="K23" s="2" t="s">
-        <v>25</v>
-      </c>
       <c r="L23" s="2">
         <v>1</v>
       </c>
       <c r="M23" s="2">
         <v>1</v>
       </c>
-      <c r="N23" s="2"/>
+      <c r="N23" s="2">
+        <v>1</v>
+      </c>
       <c r="O23" s="2"/>
       <c r="P23" s="2"/>
       <c r="Q23" s="2"/>
@@ -2441,8 +2463,9 @@
       <c r="T23" s="2"/>
       <c r="U23" s="2"/>
       <c r="V23" s="2"/>
-    </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W23" s="2"/>
+    </row>
+    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>23</v>
       </c>
@@ -2465,24 +2488,23 @@
         <v>12</v>
       </c>
       <c r="H24" s="2">
-        <v>1</v>
-      </c>
-      <c r="I24" s="2">
         <v>2.4</v>
       </c>
+      <c r="I24" s="2" t="s">
+        <v>77</v>
+      </c>
       <c r="J24" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="K24" s="2" t="s">
-        <v>77</v>
-      </c>
       <c r="L24" s="2">
         <v>1</v>
       </c>
       <c r="M24" s="2">
         <v>1</v>
       </c>
-      <c r="N24" s="2"/>
+      <c r="N24" s="2">
+        <v>1</v>
+      </c>
       <c r="O24" s="2"/>
       <c r="P24" s="2"/>
       <c r="Q24" s="2"/>
@@ -2491,8 +2513,9 @@
       <c r="T24" s="2"/>
       <c r="U24" s="2"/>
       <c r="V24" s="2"/>
-    </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W24" s="2"/>
+    </row>
+    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>24</v>
       </c>
@@ -2515,22 +2538,21 @@
         <v>12</v>
       </c>
       <c r="H25" s="2">
-        <v>1</v>
-      </c>
-      <c r="I25" s="2">
         <v>6.6</v>
       </c>
+      <c r="I25" s="2"/>
       <c r="J25" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="K25" s="2"/>
       <c r="L25" s="2">
         <v>1</v>
       </c>
       <c r="M25" s="2">
         <v>1</v>
       </c>
-      <c r="N25" s="2"/>
+      <c r="N25" s="2">
+        <v>1</v>
+      </c>
       <c r="O25" s="2"/>
       <c r="P25" s="2"/>
       <c r="Q25" s="2"/>
@@ -2539,8 +2561,9 @@
       <c r="T25" s="2"/>
       <c r="U25" s="2"/>
       <c r="V25" s="2"/>
-    </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W25" s="2"/>
+    </row>
+    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>25</v>
       </c>
@@ -2563,22 +2586,21 @@
         <v>12</v>
       </c>
       <c r="H26" s="2">
-        <v>4</v>
-      </c>
-      <c r="I26" s="2">
         <v>6.6</v>
       </c>
+      <c r="I26" s="2"/>
       <c r="J26" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="K26" s="2"/>
       <c r="L26" s="2">
         <v>4</v>
       </c>
       <c r="M26" s="2">
         <v>4</v>
       </c>
-      <c r="N26" s="2"/>
+      <c r="N26" s="2">
+        <v>4</v>
+      </c>
       <c r="O26" s="2"/>
       <c r="P26" s="2"/>
       <c r="Q26" s="2"/>
@@ -2587,8 +2609,9 @@
       <c r="T26" s="2"/>
       <c r="U26" s="2"/>
       <c r="V26" s="2"/>
-    </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W26" s="2"/>
+    </row>
+    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>26</v>
       </c>
@@ -2609,23 +2632,22 @@
         <v>103</v>
       </c>
       <c r="H27" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2"/>
+      <c r="L27" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="I27" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="J27" s="2"/>
-      <c r="K27" s="2"/>
-      <c r="L27" s="2">
-        <v>2</v>
-      </c>
       <c r="M27" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N27" s="2">
         <v>1</v>
       </c>
-      <c r="O27" s="2"/>
+      <c r="O27" s="2">
+        <v>1</v>
+      </c>
       <c r="P27" s="2"/>
       <c r="Q27" s="2"/>
       <c r="R27" s="2"/>
@@ -2633,8 +2655,9 @@
       <c r="T27" s="2"/>
       <c r="U27" s="2"/>
       <c r="V27" s="2"/>
-    </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W27" s="2"/>
+    </row>
+    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>27</v>
       </c>
@@ -2657,34 +2680,34 @@
         <v>55</v>
       </c>
       <c r="H28" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="I28" s="2"/>
+      <c r="J28" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="L28" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="I28" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="J28" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="K28" s="2"/>
-      <c r="L28" s="2">
+      <c r="M28" s="2">
         <v>4</v>
       </c>
-      <c r="M28" s="2">
-        <v>1</v>
-      </c>
-      <c r="N28" s="2"/>
+      <c r="N28" s="2">
+        <v>1</v>
+      </c>
       <c r="O28" s="2"/>
       <c r="P28" s="2"/>
       <c r="Q28" s="2"/>
       <c r="R28" s="2"/>
-      <c r="S28" s="2">
+      <c r="S28" s="2"/>
+      <c r="T28" s="2">
         <v>3</v>
       </c>
-      <c r="T28" s="2"/>
       <c r="U28" s="2"/>
       <c r="V28" s="2"/>
-    </row>
-    <row r="29" spans="1:22" ht="30" x14ac:dyDescent="0.25">
+      <c r="W28" s="2"/>
+    </row>
+    <row r="29" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>28</v>
       </c>
@@ -2707,22 +2730,21 @@
         <v>12</v>
       </c>
       <c r="H29" s="2">
-        <v>1</v>
-      </c>
-      <c r="I29" s="2">
         <v>6.6</v>
       </c>
+      <c r="I29" s="2"/>
       <c r="J29" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="K29" s="2"/>
       <c r="L29" s="2">
         <v>1</v>
       </c>
       <c r="M29" s="2">
         <v>1</v>
       </c>
-      <c r="N29" s="2"/>
+      <c r="N29" s="2">
+        <v>1</v>
+      </c>
       <c r="O29" s="2"/>
       <c r="P29" s="2"/>
       <c r="Q29" s="2"/>
@@ -2731,8 +2753,9 @@
       <c r="T29" s="2"/>
       <c r="U29" s="2"/>
       <c r="V29" s="2"/>
-    </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W29" s="2"/>
+    </row>
+    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>29</v>
       </c>
@@ -2754,37 +2777,37 @@
       <c r="G30" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="H30" s="2" t="s">
+      <c r="H30" s="2">
+        <v>3.7</v>
+      </c>
+      <c r="I30" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="J30" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="L30" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="I30" s="2">
-        <v>3.7</v>
-      </c>
-      <c r="J30" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="K30" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="L30" s="2">
+      <c r="M30" s="2">
         <v>3</v>
       </c>
-      <c r="M30" s="2">
-        <v>1</v>
-      </c>
-      <c r="N30" s="2"/>
+      <c r="N30" s="2">
+        <v>1</v>
+      </c>
       <c r="O30" s="2"/>
       <c r="P30" s="2"/>
       <c r="Q30" s="2"/>
       <c r="R30" s="2"/>
-      <c r="S30" s="2">
-        <v>2</v>
-      </c>
-      <c r="T30" s="2"/>
+      <c r="S30" s="2"/>
+      <c r="T30" s="2">
+        <v>2</v>
+      </c>
       <c r="U30" s="2"/>
       <c r="V30" s="2"/>
-    </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W30" s="2"/>
+    </row>
+    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>30</v>
       </c>
@@ -2806,26 +2829,25 @@
       <c r="G31" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="H31" s="2" t="s">
+      <c r="H31" s="2">
+        <v>3.7</v>
+      </c>
+      <c r="I31" s="2"/>
+      <c r="J31" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="L31" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="I31" s="2">
-        <v>3.7</v>
-      </c>
-      <c r="J31" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="K31" s="2"/>
-      <c r="L31" s="2">
-        <v>2</v>
-      </c>
       <c r="M31" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N31" s="2">
         <v>1</v>
       </c>
-      <c r="O31" s="2"/>
+      <c r="O31" s="2">
+        <v>1</v>
+      </c>
       <c r="P31" s="2"/>
       <c r="Q31" s="2"/>
       <c r="R31" s="2"/>
@@ -2833,8 +2855,9 @@
       <c r="T31" s="2"/>
       <c r="U31" s="2"/>
       <c r="V31" s="2"/>
-    </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W31" s="2"/>
+    </row>
+    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>31</v>
       </c>
@@ -2857,24 +2880,23 @@
         <v>12</v>
       </c>
       <c r="H32" s="2">
-        <v>2</v>
-      </c>
-      <c r="I32" s="2">
         <v>7</v>
       </c>
+      <c r="I32" s="2" t="s">
+        <v>119</v>
+      </c>
       <c r="J32" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="K32" s="2" t="s">
-        <v>119</v>
-      </c>
       <c r="L32" s="2">
         <v>2</v>
       </c>
       <c r="M32" s="2">
         <v>2</v>
       </c>
-      <c r="N32" s="2"/>
+      <c r="N32" s="2">
+        <v>2</v>
+      </c>
       <c r="O32" s="2"/>
       <c r="P32" s="2"/>
       <c r="Q32" s="2"/>
@@ -2883,8 +2905,9 @@
       <c r="T32" s="2"/>
       <c r="U32" s="2"/>
       <c r="V32" s="2"/>
-    </row>
-    <row r="33" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W32" s="2"/>
+    </row>
+    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>32</v>
       </c>
@@ -2907,23 +2930,20 @@
         <v>122</v>
       </c>
       <c r="H33" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="I33" s="2"/>
+      <c r="J33" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="L33" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="I33" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="J33" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="K33" s="2"/>
-      <c r="L33" s="7">
+      <c r="M33" s="7">
         <v>7</v>
       </c>
-      <c r="M33" s="2">
-        <v>2</v>
-      </c>
       <c r="N33" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O33" s="2">
         <v>1</v>
@@ -2934,15 +2954,18 @@
       <c r="Q33" s="2">
         <v>1</v>
       </c>
-      <c r="R33" s="2"/>
+      <c r="R33" s="2">
+        <v>1</v>
+      </c>
       <c r="S33" s="2"/>
       <c r="T33" s="2"/>
-      <c r="U33" s="2">
-        <v>1</v>
-      </c>
-      <c r="V33" s="2"/>
-    </row>
-    <row r="34" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="U33" s="2"/>
+      <c r="V33" s="2">
+        <v>1</v>
+      </c>
+      <c r="W33" s="2"/>
+    </row>
+    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>33</v>
       </c>
@@ -2965,24 +2988,23 @@
         <v>12</v>
       </c>
       <c r="H34" s="2">
-        <v>1</v>
-      </c>
-      <c r="I34" s="2">
         <v>6</v>
       </c>
+      <c r="I34" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="J34" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="K34" s="2" t="s">
-        <v>28</v>
-      </c>
       <c r="L34" s="2">
         <v>1</v>
       </c>
       <c r="M34" s="2">
         <v>1</v>
       </c>
-      <c r="N34" s="2"/>
+      <c r="N34" s="2">
+        <v>1</v>
+      </c>
       <c r="O34" s="2"/>
       <c r="P34" s="2"/>
       <c r="Q34" s="2"/>
@@ -2991,8 +3013,9 @@
       <c r="T34" s="2"/>
       <c r="U34" s="2"/>
       <c r="V34" s="2"/>
-    </row>
-    <row r="35" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W34" s="2"/>
+    </row>
+    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>34</v>
       </c>
@@ -3015,36 +3038,36 @@
         <v>55</v>
       </c>
       <c r="H35" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="I35" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="J35" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="L35" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="I35" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="J35" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="K35" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="L35" s="2">
+      <c r="M35" s="2">
         <v>3</v>
       </c>
-      <c r="M35" s="2">
-        <v>1</v>
-      </c>
-      <c r="N35" s="2"/>
+      <c r="N35" s="2">
+        <v>1</v>
+      </c>
       <c r="O35" s="2"/>
       <c r="P35" s="2"/>
       <c r="Q35" s="2"/>
       <c r="R35" s="2"/>
-      <c r="S35" s="2">
-        <v>2</v>
-      </c>
-      <c r="T35" s="2"/>
+      <c r="S35" s="2"/>
+      <c r="T35" s="2">
+        <v>2</v>
+      </c>
       <c r="U35" s="2"/>
       <c r="V35" s="2"/>
-    </row>
-    <row r="36" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W35" s="2"/>
+    </row>
+    <row r="36" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>35</v>
       </c>
@@ -3066,89 +3089,90 @@
       <c r="G36" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="H36" s="2">
-        <v>1</v>
-      </c>
-      <c r="I36" s="2" t="s">
+      <c r="H36" s="2" t="s">
         <v>107</v>
       </c>
+      <c r="I36" s="2"/>
       <c r="J36" s="2"/>
-      <c r="K36" s="2"/>
-      <c r="L36" s="7">
+      <c r="L36" s="2">
+        <v>1</v>
+      </c>
+      <c r="M36" s="7">
         <v>5</v>
       </c>
-      <c r="M36" s="2">
-        <v>1</v>
-      </c>
       <c r="N36" s="2">
         <v>1</v>
       </c>
       <c r="O36" s="2">
         <v>1</v>
       </c>
-      <c r="P36" s="2"/>
-      <c r="Q36" s="2">
-        <v>1</v>
-      </c>
-      <c r="R36" s="2"/>
+      <c r="P36" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q36" s="2"/>
+      <c r="R36" s="2">
+        <v>1</v>
+      </c>
       <c r="S36" s="2"/>
       <c r="T36" s="2"/>
-      <c r="U36" s="2">
-        <v>1</v>
-      </c>
-      <c r="V36" s="2"/>
-    </row>
-    <row r="37" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A37" s="2">
+      <c r="U36" s="2"/>
+      <c r="V36" s="2">
+        <v>1</v>
+      </c>
+      <c r="W36" s="2"/>
+    </row>
+    <row r="37" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A37" s="13">
         <v>36</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="B37" s="13" t="s">
         <v>135</v>
       </c>
-      <c r="C37" s="2">
+      <c r="C37" s="13">
         <v>3800</v>
       </c>
-      <c r="D37" s="2" t="s">
+      <c r="D37" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="E37" s="2" t="s">
+      <c r="E37" s="13" t="s">
         <v>134</v>
       </c>
-      <c r="F37" s="2" t="s">
+      <c r="F37" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="G37" s="2" t="s">
+      <c r="G37" s="13" t="s">
         <v>136</v>
       </c>
-      <c r="H37" s="2">
-        <v>1</v>
-      </c>
-      <c r="I37" s="2">
+      <c r="H37" s="13">
         <v>50</v>
       </c>
-      <c r="J37" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="K37" s="2"/>
-      <c r="L37" s="2">
-        <v>2</v>
-      </c>
-      <c r="M37" s="2"/>
+      <c r="I37" s="13"/>
+      <c r="J37" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="K37" s="14"/>
+      <c r="L37" s="13">
+        <v>1</v>
+      </c>
+      <c r="M37" s="13">
+        <v>2</v>
+      </c>
       <c r="N37" s="2"/>
-      <c r="O37" s="2">
-        <v>1</v>
-      </c>
-      <c r="P37" s="2"/>
+      <c r="O37" s="2"/>
+      <c r="P37" s="2">
+        <v>1</v>
+      </c>
       <c r="Q37" s="2"/>
       <c r="R37" s="2"/>
       <c r="S37" s="2"/>
-      <c r="T37" s="2">
-        <v>1</v>
-      </c>
-      <c r="U37" s="2"/>
+      <c r="T37" s="2"/>
+      <c r="U37" s="2">
+        <v>1</v>
+      </c>
       <c r="V37" s="2"/>
-    </row>
-    <row r="38" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W37" s="2"/>
+    </row>
+    <row r="38" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>37</v>
       </c>
@@ -3169,32 +3193,32 @@
         <v>45</v>
       </c>
       <c r="H38" s="2">
-        <v>1</v>
-      </c>
-      <c r="I38" s="2">
         <v>50</v>
       </c>
+      <c r="I38" s="2"/>
       <c r="J38" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="K38" s="2"/>
       <c r="L38" s="2">
         <v>1</v>
       </c>
-      <c r="M38" s="2"/>
+      <c r="M38" s="2">
+        <v>1</v>
+      </c>
       <c r="N38" s="2"/>
       <c r="O38" s="2"/>
       <c r="P38" s="2"/>
       <c r="Q38" s="2"/>
       <c r="R38" s="2"/>
       <c r="S38" s="2"/>
-      <c r="T38" s="2">
-        <v>1</v>
-      </c>
-      <c r="U38" s="2"/>
+      <c r="T38" s="2"/>
+      <c r="U38" s="2">
+        <v>1</v>
+      </c>
       <c r="V38" s="2"/>
-    </row>
-    <row r="39" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W38" s="2"/>
+    </row>
+    <row r="39" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>38</v>
       </c>
@@ -3217,82 +3241,83 @@
         <v>141</v>
       </c>
       <c r="H39" s="2">
+        <v>120</v>
+      </c>
+      <c r="I39" s="2"/>
+      <c r="J39" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="L39" s="2">
         <v>8</v>
       </c>
-      <c r="I39" s="2">
-        <v>120</v>
-      </c>
-      <c r="J39" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="K39" s="2"/>
-      <c r="L39" s="7">
+      <c r="M39" s="7">
         <v>8</v>
       </c>
-      <c r="M39" s="2"/>
       <c r="N39" s="2"/>
       <c r="O39" s="2"/>
       <c r="P39" s="2"/>
       <c r="Q39" s="2"/>
-      <c r="R39" s="2">
+      <c r="R39" s="2"/>
+      <c r="S39" s="2">
         <v>8</v>
       </c>
-      <c r="S39" s="2"/>
       <c r="T39" s="2"/>
       <c r="U39" s="2"/>
       <c r="V39" s="2"/>
-    </row>
-    <row r="40" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A40" s="2">
+      <c r="W39" s="2"/>
+    </row>
+    <row r="40" spans="1:23" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="15">
         <v>39</v>
       </c>
-      <c r="B40" s="2" t="s">
+      <c r="B40" s="15" t="s">
         <v>143</v>
       </c>
-      <c r="C40" s="2">
+      <c r="C40" s="15">
         <v>1219</v>
       </c>
-      <c r="D40" s="2" t="s">
+      <c r="D40" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="E40" s="2" t="s">
+      <c r="E40" s="15" t="s">
         <v>142</v>
       </c>
-      <c r="F40" s="2" t="s">
+      <c r="F40" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="G40" s="2" t="s">
+      <c r="G40" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="H40" s="2">
-        <v>2</v>
-      </c>
-      <c r="I40" s="2" t="s">
+      <c r="H40" s="15" t="s">
         <v>144</v>
       </c>
-      <c r="J40" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="K40" s="2"/>
-      <c r="L40" s="2">
+      <c r="I40" s="15"/>
+      <c r="J40" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="K40" s="16"/>
+      <c r="L40" s="15">
+        <v>2</v>
+      </c>
+      <c r="M40" s="15">
         <v>4</v>
       </c>
-      <c r="M40" s="2">
-        <v>2</v>
-      </c>
-      <c r="N40" s="2"/>
-      <c r="O40" s="2"/>
-      <c r="P40" s="2"/>
-      <c r="Q40" s="2"/>
-      <c r="R40" s="2"/>
-      <c r="S40" s="2">
-        <v>2</v>
-      </c>
-      <c r="T40" s="2"/>
-      <c r="U40" s="2"/>
-      <c r="V40" s="2"/>
-    </row>
-    <row r="41" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="N40" s="15">
+        <v>2</v>
+      </c>
+      <c r="O40" s="15"/>
+      <c r="P40" s="15"/>
+      <c r="Q40" s="15"/>
+      <c r="R40" s="15"/>
+      <c r="S40" s="15"/>
+      <c r="T40" s="15">
+        <v>2</v>
+      </c>
+      <c r="U40" s="15"/>
+      <c r="V40" s="15"/>
+      <c r="W40" s="15"/>
+    </row>
+    <row r="41" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>40</v>
       </c>
@@ -3314,37 +3339,37 @@
       <c r="G41" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="H41" s="2">
-        <v>1</v>
+      <c r="H41" s="2" t="s">
+        <v>148</v>
       </c>
       <c r="I41" s="2" t="s">
-        <v>148</v>
+        <v>28</v>
       </c>
       <c r="J41" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="K41" s="2" t="s">
-        <v>28</v>
-      </c>
       <c r="L41" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M41" s="2">
-        <v>1</v>
-      </c>
-      <c r="N41" s="2"/>
+        <v>2</v>
+      </c>
+      <c r="N41" s="2">
+        <v>1</v>
+      </c>
       <c r="O41" s="2"/>
       <c r="P41" s="2"/>
       <c r="Q41" s="2"/>
       <c r="R41" s="2"/>
       <c r="S41" s="2"/>
       <c r="T41" s="2"/>
-      <c r="U41" s="2">
-        <v>1</v>
-      </c>
-      <c r="V41" s="2"/>
-    </row>
-    <row r="42" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="U41" s="2"/>
+      <c r="V41" s="2">
+        <v>1</v>
+      </c>
+      <c r="W41" s="2"/>
+    </row>
+    <row r="42" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>41</v>
       </c>
@@ -3367,32 +3392,32 @@
         <v>65</v>
       </c>
       <c r="H42" s="2">
-        <v>2</v>
-      </c>
-      <c r="I42" s="2">
         <v>9</v>
       </c>
+      <c r="I42" s="2"/>
       <c r="J42" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="K42" s="2"/>
       <c r="L42" s="2">
         <v>2</v>
       </c>
-      <c r="M42" s="2"/>
+      <c r="M42" s="2">
+        <v>2</v>
+      </c>
       <c r="N42" s="2"/>
       <c r="O42" s="2"/>
       <c r="P42" s="2"/>
       <c r="Q42" s="2"/>
       <c r="R42" s="2"/>
-      <c r="S42" s="2">
-        <v>2</v>
-      </c>
-      <c r="T42" s="2"/>
+      <c r="S42" s="2"/>
+      <c r="T42" s="2">
+        <v>2</v>
+      </c>
       <c r="U42" s="2"/>
       <c r="V42" s="2"/>
-    </row>
-    <row r="43" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W42" s="2"/>
+    </row>
+    <row r="43" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>42</v>
       </c>
@@ -3414,21 +3439,20 @@
       <c r="G43" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="H43" s="2">
-        <v>2</v>
-      </c>
-      <c r="I43" s="2" t="s">
+      <c r="H43" s="2" t="s">
         <v>107</v>
       </c>
+      <c r="I43" s="2"/>
       <c r="J43" s="2"/>
-      <c r="K43" s="2"/>
       <c r="L43" s="2">
         <v>2</v>
       </c>
       <c r="M43" s="2">
         <v>2</v>
       </c>
-      <c r="N43" s="2"/>
+      <c r="N43" s="2">
+        <v>2</v>
+      </c>
       <c r="O43" s="2"/>
       <c r="P43" s="2"/>
       <c r="Q43" s="2"/>
@@ -3437,8 +3461,9 @@
       <c r="T43" s="2"/>
       <c r="U43" s="2"/>
       <c r="V43" s="2"/>
-    </row>
-    <row r="44" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W43" s="2"/>
+    </row>
+    <row r="44" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>43</v>
       </c>
@@ -3461,24 +3486,23 @@
         <v>12</v>
       </c>
       <c r="H44" s="2">
-        <v>1</v>
-      </c>
-      <c r="I44" s="2">
         <v>6.6</v>
       </c>
+      <c r="I44" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="J44" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="K44" s="2" t="s">
-        <v>25</v>
-      </c>
       <c r="L44" s="2">
         <v>1</v>
       </c>
       <c r="M44" s="2">
         <v>1</v>
       </c>
-      <c r="N44" s="2"/>
+      <c r="N44" s="2">
+        <v>1</v>
+      </c>
       <c r="O44" s="2"/>
       <c r="P44" s="2"/>
       <c r="Q44" s="2"/>
@@ -3487,8 +3511,9 @@
       <c r="T44" s="2"/>
       <c r="U44" s="2"/>
       <c r="V44" s="2"/>
-    </row>
-    <row r="45" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W44" s="2"/>
+    </row>
+    <row r="45" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>44</v>
       </c>
@@ -3511,34 +3536,34 @@
         <v>157</v>
       </c>
       <c r="H45" s="2">
-        <v>1</v>
-      </c>
-      <c r="I45" s="2">
         <v>7.4</v>
       </c>
+      <c r="I45" s="2"/>
       <c r="J45" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="K45" s="2"/>
       <c r="L45" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M45" s="2">
-        <v>1</v>
-      </c>
-      <c r="N45" s="2"/>
+        <v>2</v>
+      </c>
+      <c r="N45" s="2">
+        <v>1</v>
+      </c>
       <c r="O45" s="2"/>
-      <c r="P45" s="2">
-        <v>1</v>
-      </c>
-      <c r="Q45" s="2"/>
+      <c r="P45" s="2"/>
+      <c r="Q45" s="2">
+        <v>1</v>
+      </c>
       <c r="R45" s="2"/>
       <c r="S45" s="2"/>
       <c r="T45" s="2"/>
       <c r="U45" s="2"/>
       <c r="V45" s="2"/>
-    </row>
-    <row r="46" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W45" s="2"/>
+    </row>
+    <row r="46" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>45</v>
       </c>
@@ -3561,32 +3586,32 @@
         <v>65</v>
       </c>
       <c r="H46" s="2">
-        <v>2</v>
-      </c>
-      <c r="I46" s="2">
         <v>10</v>
       </c>
+      <c r="I46" s="2"/>
       <c r="J46" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="K46" s="2"/>
       <c r="L46" s="2">
         <v>2</v>
       </c>
-      <c r="M46" s="2"/>
+      <c r="M46" s="2">
+        <v>2</v>
+      </c>
       <c r="N46" s="2"/>
       <c r="O46" s="2"/>
       <c r="P46" s="2"/>
       <c r="Q46" s="2"/>
       <c r="R46" s="2"/>
-      <c r="S46" s="2">
-        <v>2</v>
-      </c>
-      <c r="T46" s="2"/>
+      <c r="S46" s="2"/>
+      <c r="T46" s="2">
+        <v>2</v>
+      </c>
       <c r="U46" s="2"/>
       <c r="V46" s="2"/>
-    </row>
-    <row r="47" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W46" s="2"/>
+    </row>
+    <row r="47" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <v>46</v>
       </c>
@@ -3607,32 +3632,32 @@
         <v>42</v>
       </c>
       <c r="H47" s="2">
-        <v>1</v>
-      </c>
-      <c r="I47" s="2">
         <v>7.4</v>
       </c>
+      <c r="I47" s="2"/>
       <c r="J47" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="K47" s="2"/>
       <c r="L47" s="2">
         <v>1</v>
       </c>
-      <c r="M47" s="2"/>
+      <c r="M47" s="2">
+        <v>1</v>
+      </c>
       <c r="N47" s="2"/>
       <c r="O47" s="2"/>
-      <c r="P47" s="2">
-        <v>1</v>
-      </c>
-      <c r="Q47" s="2"/>
+      <c r="P47" s="2"/>
+      <c r="Q47" s="2">
+        <v>1</v>
+      </c>
       <c r="R47" s="2"/>
       <c r="S47" s="2"/>
       <c r="T47" s="2"/>
       <c r="U47" s="2"/>
       <c r="V47" s="2"/>
-    </row>
-    <row r="48" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W47" s="2"/>
+    </row>
+    <row r="48" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
         <v>47</v>
       </c>
@@ -3655,22 +3680,21 @@
         <v>12</v>
       </c>
       <c r="H48" s="2">
-        <v>1</v>
-      </c>
-      <c r="I48" s="2">
         <v>3.7</v>
       </c>
+      <c r="I48" s="2"/>
       <c r="J48" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="K48" s="2"/>
       <c r="L48" s="2">
         <v>1</v>
       </c>
       <c r="M48" s="2">
         <v>1</v>
       </c>
-      <c r="N48" s="2"/>
+      <c r="N48" s="2">
+        <v>1</v>
+      </c>
       <c r="O48" s="2"/>
       <c r="P48" s="2"/>
       <c r="Q48" s="2"/>
@@ -3679,8 +3703,9 @@
       <c r="T48" s="2"/>
       <c r="U48" s="2"/>
       <c r="V48" s="2"/>
-    </row>
-    <row r="49" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W48" s="2"/>
+    </row>
+    <row r="49" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <v>48</v>
       </c>
@@ -3703,22 +3728,21 @@
         <v>12</v>
       </c>
       <c r="H49" s="2">
-        <v>1</v>
-      </c>
-      <c r="I49" s="2">
         <v>7.4</v>
       </c>
+      <c r="I49" s="2"/>
       <c r="J49" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="K49" s="2"/>
       <c r="L49" s="2">
         <v>1</v>
       </c>
       <c r="M49" s="2">
         <v>1</v>
       </c>
-      <c r="N49" s="2"/>
+      <c r="N49" s="2">
+        <v>1</v>
+      </c>
       <c r="O49" s="2"/>
       <c r="P49" s="2"/>
       <c r="Q49" s="2"/>
@@ -3727,8 +3751,9 @@
       <c r="T49" s="2"/>
       <c r="U49" s="2"/>
       <c r="V49" s="2"/>
-    </row>
-    <row r="50" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W49" s="2"/>
+    </row>
+    <row r="50" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
         <v>49</v>
       </c>
@@ -3750,31 +3775,31 @@
       <c r="G50" s="6" t="s">
         <v>141</v>
       </c>
-      <c r="H50" s="2">
-        <v>2</v>
-      </c>
-      <c r="I50" s="2" t="s">
+      <c r="H50" s="2" t="s">
         <v>107</v>
       </c>
+      <c r="I50" s="2"/>
       <c r="J50" s="2"/>
-      <c r="K50" s="2"/>
       <c r="L50" s="2">
         <v>2</v>
       </c>
-      <c r="M50" s="2"/>
+      <c r="M50" s="2">
+        <v>2</v>
+      </c>
       <c r="N50" s="2"/>
       <c r="O50" s="2"/>
       <c r="P50" s="2"/>
       <c r="Q50" s="2"/>
-      <c r="R50" s="2">
-        <v>2</v>
-      </c>
-      <c r="S50" s="2"/>
+      <c r="R50" s="2"/>
+      <c r="S50" s="2">
+        <v>2</v>
+      </c>
       <c r="T50" s="2"/>
       <c r="U50" s="2"/>
       <c r="V50" s="2"/>
-    </row>
-    <row r="51" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W50" s="2"/>
+    </row>
+    <row r="51" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
         <v>50</v>
       </c>
@@ -3797,22 +3822,21 @@
         <v>12</v>
       </c>
       <c r="H51" s="2">
-        <v>1</v>
-      </c>
-      <c r="I51" s="2">
         <v>6</v>
       </c>
+      <c r="I51" s="2"/>
       <c r="J51" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="K51" s="2"/>
       <c r="L51" s="2">
         <v>1</v>
       </c>
       <c r="M51" s="2">
         <v>1</v>
       </c>
-      <c r="N51" s="2"/>
+      <c r="N51" s="2">
+        <v>1</v>
+      </c>
       <c r="O51" s="2"/>
       <c r="P51" s="2"/>
       <c r="Q51" s="2"/>
@@ -3821,8 +3845,9 @@
       <c r="T51" s="2"/>
       <c r="U51" s="2"/>
       <c r="V51" s="2"/>
-    </row>
-    <row r="52" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W51" s="2"/>
+    </row>
+    <row r="52" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
         <v>51</v>
       </c>
@@ -3845,32 +3870,32 @@
         <v>65</v>
       </c>
       <c r="H52" s="2">
-        <v>2</v>
-      </c>
-      <c r="I52" s="2">
         <v>14</v>
       </c>
+      <c r="I52" s="2"/>
       <c r="J52" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="K52" s="2"/>
       <c r="L52" s="2">
         <v>2</v>
       </c>
-      <c r="M52" s="2"/>
+      <c r="M52" s="2">
+        <v>2</v>
+      </c>
       <c r="N52" s="2"/>
       <c r="O52" s="2"/>
       <c r="P52" s="2"/>
       <c r="Q52" s="2"/>
       <c r="R52" s="2"/>
-      <c r="S52" s="2">
-        <v>2</v>
-      </c>
-      <c r="T52" s="2"/>
+      <c r="S52" s="2"/>
+      <c r="T52" s="2">
+        <v>2</v>
+      </c>
       <c r="U52" s="2"/>
       <c r="V52" s="2"/>
-    </row>
-    <row r="53" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W52" s="2"/>
+    </row>
+    <row r="53" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
         <v>52</v>
       </c>
@@ -3892,31 +3917,31 @@
       <c r="G53" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="H53" s="2">
-        <v>2</v>
-      </c>
-      <c r="I53" s="2" t="s">
+      <c r="H53" s="2" t="s">
         <v>107</v>
       </c>
+      <c r="I53" s="2"/>
       <c r="J53" s="2"/>
-      <c r="K53" s="2"/>
       <c r="L53" s="2">
         <v>2</v>
       </c>
-      <c r="M53" s="2"/>
+      <c r="M53" s="2">
+        <v>2</v>
+      </c>
       <c r="N53" s="2"/>
       <c r="O53" s="2"/>
       <c r="P53" s="2"/>
       <c r="Q53" s="2"/>
       <c r="R53" s="2"/>
-      <c r="S53" s="2">
-        <v>2</v>
-      </c>
-      <c r="T53" s="2"/>
+      <c r="S53" s="2"/>
+      <c r="T53" s="2">
+        <v>2</v>
+      </c>
       <c r="U53" s="2"/>
       <c r="V53" s="2"/>
-    </row>
-    <row r="54" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W53" s="2"/>
+    </row>
+    <row r="54" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
         <v>53</v>
       </c>
@@ -3939,32 +3964,32 @@
         <v>65</v>
       </c>
       <c r="H54" s="2">
-        <v>2</v>
-      </c>
-      <c r="I54" s="2">
         <v>18</v>
       </c>
+      <c r="I54" s="2"/>
       <c r="J54" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="K54" s="2"/>
       <c r="L54" s="2">
         <v>2</v>
       </c>
-      <c r="M54" s="2"/>
+      <c r="M54" s="2">
+        <v>2</v>
+      </c>
       <c r="N54" s="2"/>
       <c r="O54" s="2"/>
       <c r="P54" s="2"/>
       <c r="Q54" s="2"/>
       <c r="R54" s="2"/>
-      <c r="S54" s="2">
-        <v>2</v>
-      </c>
-      <c r="T54" s="2"/>
+      <c r="S54" s="2"/>
+      <c r="T54" s="2">
+        <v>2</v>
+      </c>
       <c r="U54" s="2"/>
       <c r="V54" s="2"/>
-    </row>
-    <row r="55" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W54" s="2"/>
+    </row>
+    <row r="55" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
         <v>54</v>
       </c>
@@ -3987,32 +4012,32 @@
         <v>65</v>
       </c>
       <c r="H55" s="2">
-        <v>2</v>
-      </c>
-      <c r="I55" s="2">
         <v>8</v>
       </c>
+      <c r="I55" s="2"/>
       <c r="J55" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="K55" s="2"/>
       <c r="L55" s="2">
         <v>2</v>
       </c>
-      <c r="M55" s="2"/>
+      <c r="M55" s="2">
+        <v>2</v>
+      </c>
       <c r="N55" s="2"/>
       <c r="O55" s="2"/>
       <c r="P55" s="2"/>
       <c r="Q55" s="2"/>
       <c r="R55" s="2"/>
-      <c r="S55" s="2">
-        <v>2</v>
-      </c>
-      <c r="T55" s="2"/>
+      <c r="S55" s="2"/>
+      <c r="T55" s="2">
+        <v>2</v>
+      </c>
       <c r="U55" s="2"/>
       <c r="V55" s="2"/>
-    </row>
-    <row r="56" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W55" s="2"/>
+    </row>
+    <row r="56" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
         <v>55</v>
       </c>
@@ -4035,32 +4060,32 @@
         <v>65</v>
       </c>
       <c r="H56" s="2">
-        <v>2</v>
-      </c>
-      <c r="I56" s="2">
         <v>18</v>
       </c>
+      <c r="I56" s="2"/>
       <c r="J56" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="K56" s="2"/>
       <c r="L56" s="2">
         <v>2</v>
       </c>
-      <c r="M56" s="2"/>
+      <c r="M56" s="2">
+        <v>2</v>
+      </c>
       <c r="N56" s="2"/>
       <c r="O56" s="2"/>
       <c r="P56" s="2"/>
       <c r="Q56" s="2"/>
       <c r="R56" s="2"/>
-      <c r="S56" s="2">
-        <v>2</v>
-      </c>
-      <c r="T56" s="2"/>
+      <c r="S56" s="2"/>
+      <c r="T56" s="2">
+        <v>2</v>
+      </c>
       <c r="U56" s="2"/>
       <c r="V56" s="2"/>
-    </row>
-    <row r="57" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W56" s="2"/>
+    </row>
+    <row r="57" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
         <v>56</v>
       </c>
@@ -4083,32 +4108,32 @@
         <v>65</v>
       </c>
       <c r="H57" s="2">
-        <v>2</v>
-      </c>
-      <c r="I57" s="2">
         <v>8</v>
       </c>
+      <c r="I57" s="2"/>
       <c r="J57" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="K57" s="2"/>
       <c r="L57" s="2">
         <v>2</v>
       </c>
-      <c r="M57" s="2"/>
+      <c r="M57" s="2">
+        <v>2</v>
+      </c>
       <c r="N57" s="2"/>
       <c r="O57" s="2"/>
       <c r="P57" s="2"/>
       <c r="Q57" s="2"/>
       <c r="R57" s="2"/>
-      <c r="S57" s="2">
-        <v>2</v>
-      </c>
-      <c r="T57" s="2"/>
+      <c r="S57" s="2"/>
+      <c r="T57" s="2">
+        <v>2</v>
+      </c>
       <c r="U57" s="2"/>
       <c r="V57" s="2"/>
-    </row>
-    <row r="58" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W57" s="2"/>
+    </row>
+    <row r="58" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
         <v>57</v>
       </c>
@@ -4130,35 +4155,35 @@
       <c r="G58" s="6" t="s">
         <v>185</v>
       </c>
-      <c r="H58" s="2">
-        <v>1</v>
+      <c r="H58" s="2" t="s">
+        <v>107</v>
       </c>
       <c r="I58" s="2" t="s">
-        <v>107</v>
+        <v>183</v>
       </c>
       <c r="J58" s="2"/>
-      <c r="K58" s="2" t="s">
-        <v>183</v>
-      </c>
       <c r="L58" s="2">
-        <v>2</v>
-      </c>
-      <c r="M58" s="2"/>
+        <v>1</v>
+      </c>
+      <c r="M58" s="2">
+        <v>2</v>
+      </c>
       <c r="N58" s="2"/>
       <c r="O58" s="2"/>
-      <c r="P58" s="2">
-        <v>1</v>
-      </c>
-      <c r="Q58" s="2"/>
+      <c r="P58" s="2"/>
+      <c r="Q58" s="2">
+        <v>1</v>
+      </c>
       <c r="R58" s="2"/>
-      <c r="S58" s="2">
-        <v>1</v>
-      </c>
-      <c r="T58" s="2"/>
+      <c r="S58" s="2"/>
+      <c r="T58" s="2">
+        <v>1</v>
+      </c>
       <c r="U58" s="2"/>
       <c r="V58" s="2"/>
-    </row>
-    <row r="59" spans="1:22" ht="30" x14ac:dyDescent="0.25">
+      <c r="W58" s="2"/>
+    </row>
+    <row r="59" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
         <v>58</v>
       </c>
@@ -4180,35 +4205,35 @@
       <c r="G59" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="H59" s="2" t="s">
+      <c r="H59" s="2">
+        <v>7.4</v>
+      </c>
+      <c r="I59" s="2"/>
+      <c r="J59" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="L59" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="I59" s="2">
-        <v>7.4</v>
-      </c>
-      <c r="J59" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="K59" s="2"/>
-      <c r="L59" s="7">
+      <c r="M59" s="7">
         <v>6</v>
       </c>
-      <c r="M59" s="2">
-        <v>2</v>
-      </c>
-      <c r="N59" s="2"/>
+      <c r="N59" s="2">
+        <v>2</v>
+      </c>
       <c r="O59" s="2"/>
       <c r="P59" s="2"/>
       <c r="Q59" s="2"/>
       <c r="R59" s="2"/>
-      <c r="S59" s="2">
+      <c r="S59" s="2"/>
+      <c r="T59" s="2">
         <v>4</v>
       </c>
-      <c r="T59" s="2"/>
       <c r="U59" s="2"/>
       <c r="V59" s="2"/>
-    </row>
-    <row r="60" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W59" s="2"/>
+    </row>
+    <row r="60" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
         <v>59</v>
       </c>
@@ -4231,22 +4256,21 @@
         <v>12</v>
       </c>
       <c r="H60" s="2">
-        <v>1</v>
-      </c>
-      <c r="I60" s="2">
         <v>5</v>
       </c>
+      <c r="I60" s="2"/>
       <c r="J60" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="K60" s="2"/>
       <c r="L60" s="2">
         <v>1</v>
       </c>
       <c r="M60" s="2">
         <v>1</v>
       </c>
-      <c r="N60" s="2"/>
+      <c r="N60" s="2">
+        <v>1</v>
+      </c>
       <c r="O60" s="2"/>
       <c r="P60" s="2"/>
       <c r="Q60" s="2"/>
@@ -4255,8 +4279,9 @@
       <c r="T60" s="2"/>
       <c r="U60" s="2"/>
       <c r="V60" s="2"/>
-    </row>
-    <row r="61" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W60" s="2"/>
+    </row>
+    <row r="61" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A61" s="2">
         <v>60</v>
       </c>
@@ -4278,41 +4303,41 @@
       <c r="G61" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="H61" s="2">
-        <v>1</v>
+      <c r="H61" s="2" t="s">
+        <v>192</v>
       </c>
       <c r="I61" s="2" t="s">
-        <v>192</v>
+        <v>77</v>
       </c>
       <c r="J61" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="K61" s="2" t="s">
-        <v>77</v>
-      </c>
       <c r="L61" s="2">
+        <v>1</v>
+      </c>
+      <c r="M61" s="2">
         <v>4</v>
       </c>
-      <c r="M61" s="2">
-        <v>1</v>
-      </c>
-      <c r="N61" s="2"/>
-      <c r="O61" s="2">
-        <v>1</v>
-      </c>
-      <c r="P61" s="2"/>
-      <c r="Q61" s="2">
-        <v>1</v>
-      </c>
-      <c r="R61" s="2"/>
+      <c r="N61" s="2">
+        <v>1</v>
+      </c>
+      <c r="O61" s="2"/>
+      <c r="P61" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q61" s="2"/>
+      <c r="R61" s="2">
+        <v>1</v>
+      </c>
       <c r="S61" s="2"/>
       <c r="T61" s="2"/>
-      <c r="U61" s="2">
-        <v>1</v>
-      </c>
-      <c r="V61" s="2"/>
-    </row>
-    <row r="62" spans="1:22" ht="30" x14ac:dyDescent="0.25">
+      <c r="U61" s="2"/>
+      <c r="V61" s="2">
+        <v>1</v>
+      </c>
+      <c r="W61" s="2"/>
+    </row>
+    <row r="62" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
         <v>61</v>
       </c>
@@ -4335,34 +4360,34 @@
         <v>194</v>
       </c>
       <c r="H62" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="I62" s="2"/>
+      <c r="J62" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="L62" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="I62" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="J62" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="K62" s="2"/>
-      <c r="L62" s="2">
+      <c r="M62" s="2">
         <v>4</v>
       </c>
-      <c r="M62" s="2">
-        <v>1</v>
-      </c>
-      <c r="N62" s="2"/>
+      <c r="N62" s="2">
+        <v>1</v>
+      </c>
       <c r="O62" s="2"/>
       <c r="P62" s="2"/>
       <c r="Q62" s="2"/>
       <c r="R62" s="2"/>
-      <c r="S62" s="2">
+      <c r="S62" s="2"/>
+      <c r="T62" s="2">
         <v>3</v>
       </c>
-      <c r="T62" s="2"/>
       <c r="U62" s="2"/>
       <c r="V62" s="2"/>
-    </row>
-    <row r="63" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W62" s="2"/>
+    </row>
+    <row r="63" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A63" s="2">
         <v>62</v>
       </c>
@@ -4385,32 +4410,32 @@
         <v>55</v>
       </c>
       <c r="H63" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="I63" s="2"/>
+      <c r="J63" s="2"/>
+      <c r="L63" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="I63" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="J63" s="2"/>
-      <c r="K63" s="2"/>
-      <c r="L63" s="2">
+      <c r="M63" s="2">
         <v>3</v>
       </c>
-      <c r="M63" s="2">
-        <v>1</v>
-      </c>
-      <c r="N63" s="2"/>
+      <c r="N63" s="2">
+        <v>1</v>
+      </c>
       <c r="O63" s="2"/>
       <c r="P63" s="2"/>
       <c r="Q63" s="2"/>
       <c r="R63" s="2"/>
-      <c r="S63" s="2">
-        <v>2</v>
-      </c>
-      <c r="T63" s="2"/>
+      <c r="S63" s="2"/>
+      <c r="T63" s="2">
+        <v>2</v>
+      </c>
       <c r="U63" s="2"/>
       <c r="V63" s="2"/>
-    </row>
-    <row r="64" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W63" s="2"/>
+    </row>
+    <row r="64" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A64" s="2">
         <v>63</v>
       </c>
@@ -4433,23 +4458,22 @@
         <v>198</v>
       </c>
       <c r="H64" s="2">
-        <v>4</v>
-      </c>
-      <c r="I64" s="2">
-        <v>2</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="I64" s="2"/>
       <c r="J64" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="K64" s="2"/>
       <c r="L64" s="2">
         <v>4</v>
       </c>
-      <c r="M64" s="2"/>
-      <c r="N64" s="2">
+      <c r="M64" s="2">
         <v>4</v>
       </c>
-      <c r="O64" s="2"/>
+      <c r="N64" s="2"/>
+      <c r="O64" s="2">
+        <v>4</v>
+      </c>
       <c r="P64" s="2"/>
       <c r="Q64" s="2"/>
       <c r="R64" s="2"/>
@@ -4457,8 +4481,9 @@
       <c r="T64" s="2"/>
       <c r="U64" s="2"/>
       <c r="V64" s="2"/>
-    </row>
-    <row r="65" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W64" s="2"/>
+    </row>
+    <row r="65" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
         <v>64</v>
       </c>
@@ -4481,34 +4506,34 @@
         <v>202</v>
       </c>
       <c r="H65" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="I65" s="2"/>
+      <c r="J65" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="L65" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="I65" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="J65" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="K65" s="2"/>
-      <c r="L65" s="2">
-        <v>2</v>
-      </c>
       <c r="M65" s="2">
-        <v>1</v>
-      </c>
-      <c r="N65" s="2"/>
-      <c r="O65" s="2">
-        <v>1</v>
-      </c>
-      <c r="P65" s="2"/>
+        <v>2</v>
+      </c>
+      <c r="N65" s="2">
+        <v>1</v>
+      </c>
+      <c r="O65" s="2"/>
+      <c r="P65" s="2">
+        <v>1</v>
+      </c>
       <c r="Q65" s="2"/>
       <c r="R65" s="2"/>
       <c r="S65" s="2"/>
       <c r="T65" s="2"/>
       <c r="U65" s="2"/>
       <c r="V65" s="2"/>
-    </row>
-    <row r="66" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W65" s="2"/>
+    </row>
+    <row r="66" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A66" s="2">
         <v>65</v>
       </c>
@@ -4531,24 +4556,23 @@
         <v>12</v>
       </c>
       <c r="H66" s="2">
-        <v>1</v>
-      </c>
-      <c r="I66" s="2">
         <v>6.6</v>
       </c>
+      <c r="I66" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="J66" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="K66" s="2" t="s">
-        <v>25</v>
-      </c>
       <c r="L66" s="2">
         <v>1</v>
       </c>
       <c r="M66" s="2">
         <v>1</v>
       </c>
-      <c r="N66" s="2"/>
+      <c r="N66" s="2">
+        <v>1</v>
+      </c>
       <c r="O66" s="2"/>
       <c r="P66" s="2"/>
       <c r="Q66" s="2"/>
@@ -4557,8 +4581,9 @@
       <c r="T66" s="2"/>
       <c r="U66" s="2"/>
       <c r="V66" s="2"/>
-    </row>
-    <row r="67" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W66" s="2"/>
+    </row>
+    <row r="67" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A67" s="2">
         <v>66</v>
       </c>
@@ -4581,24 +4606,23 @@
         <v>12</v>
       </c>
       <c r="H67" s="2">
-        <v>1</v>
-      </c>
-      <c r="I67" s="2">
         <v>4.8</v>
       </c>
+      <c r="I67" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="J67" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="K67" s="2" t="s">
-        <v>25</v>
-      </c>
       <c r="L67" s="2">
         <v>1</v>
       </c>
       <c r="M67" s="2">
         <v>1</v>
       </c>
-      <c r="N67" s="2"/>
+      <c r="N67" s="2">
+        <v>1</v>
+      </c>
       <c r="O67" s="2"/>
       <c r="P67" s="2"/>
       <c r="Q67" s="2"/>
@@ -4607,8 +4631,9 @@
       <c r="T67" s="2"/>
       <c r="U67" s="2"/>
       <c r="V67" s="2"/>
-    </row>
-    <row r="68" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W67" s="2"/>
+    </row>
+    <row r="68" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A68" s="2">
         <v>67</v>
       </c>
@@ -4631,34 +4656,34 @@
         <v>55</v>
       </c>
       <c r="H68" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="I68" s="2"/>
+      <c r="J68" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="L68" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="I68" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="J68" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="K68" s="2"/>
-      <c r="L68" s="2">
+      <c r="M68" s="2">
         <v>3</v>
       </c>
-      <c r="M68" s="2">
-        <v>1</v>
-      </c>
-      <c r="N68" s="2"/>
+      <c r="N68" s="2">
+        <v>1</v>
+      </c>
       <c r="O68" s="2"/>
       <c r="P68" s="2"/>
       <c r="Q68" s="2"/>
       <c r="R68" s="2"/>
-      <c r="S68" s="2">
-        <v>2</v>
-      </c>
-      <c r="T68" s="2"/>
+      <c r="S68" s="2"/>
+      <c r="T68" s="2">
+        <v>2</v>
+      </c>
       <c r="U68" s="2"/>
       <c r="V68" s="2"/>
-    </row>
-    <row r="69" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W68" s="2"/>
+    </row>
+    <row r="69" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A69" s="2">
         <v>68</v>
       </c>
@@ -4681,24 +4706,23 @@
         <v>12</v>
       </c>
       <c r="H69" s="2">
-        <v>1</v>
-      </c>
-      <c r="I69" s="2">
         <v>6</v>
       </c>
+      <c r="I69" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="J69" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="K69" s="2" t="s">
-        <v>25</v>
-      </c>
       <c r="L69" s="2">
         <v>1</v>
       </c>
       <c r="M69" s="2">
         <v>1</v>
       </c>
-      <c r="N69" s="2"/>
+      <c r="N69" s="2">
+        <v>1</v>
+      </c>
       <c r="O69" s="2"/>
       <c r="P69" s="2"/>
       <c r="Q69" s="2"/>
@@ -4707,8 +4731,9 @@
       <c r="T69" s="2"/>
       <c r="U69" s="2"/>
       <c r="V69" s="2"/>
-    </row>
-    <row r="70" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W69" s="2"/>
+    </row>
+    <row r="70" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A70" s="2">
         <v>69</v>
       </c>
@@ -4731,24 +4756,23 @@
         <v>12</v>
       </c>
       <c r="H70" s="2">
-        <v>1</v>
-      </c>
-      <c r="I70" s="2">
         <v>6.6</v>
       </c>
+      <c r="I70" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="J70" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="K70" s="2" t="s">
-        <v>25</v>
-      </c>
       <c r="L70" s="2">
         <v>1</v>
       </c>
       <c r="M70" s="2">
         <v>1</v>
       </c>
-      <c r="N70" s="2"/>
+      <c r="N70" s="2">
+        <v>1</v>
+      </c>
       <c r="O70" s="2"/>
       <c r="P70" s="2"/>
       <c r="Q70" s="2"/>
@@ -4757,8 +4781,9 @@
       <c r="T70" s="2"/>
       <c r="U70" s="2"/>
       <c r="V70" s="2"/>
-    </row>
-    <row r="71" spans="1:22" ht="30" x14ac:dyDescent="0.25">
+      <c r="W70" s="2"/>
+    </row>
+    <row r="71" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="A71" s="2">
         <v>70</v>
       </c>
@@ -4781,34 +4806,34 @@
         <v>217</v>
       </c>
       <c r="H71" s="2">
-        <v>1</v>
-      </c>
-      <c r="I71" s="2">
         <v>7.4</v>
       </c>
+      <c r="I71" s="2"/>
       <c r="J71" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="K71" s="2"/>
       <c r="L71" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M71" s="2">
-        <v>1</v>
-      </c>
-      <c r="N71" s="2"/>
+        <v>2</v>
+      </c>
+      <c r="N71" s="2">
+        <v>1</v>
+      </c>
       <c r="O71" s="2"/>
       <c r="P71" s="2"/>
       <c r="Q71" s="2"/>
       <c r="R71" s="2"/>
-      <c r="S71" s="2">
-        <v>1</v>
-      </c>
-      <c r="T71" s="2"/>
+      <c r="S71" s="2"/>
+      <c r="T71" s="2">
+        <v>1</v>
+      </c>
       <c r="U71" s="2"/>
       <c r="V71" s="2"/>
-    </row>
-    <row r="72" spans="1:22" ht="30" x14ac:dyDescent="0.25">
+      <c r="W71" s="2"/>
+    </row>
+    <row r="72" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="A72" s="2">
         <v>71</v>
       </c>
@@ -4831,34 +4856,34 @@
         <v>222</v>
       </c>
       <c r="H72" s="2">
-        <v>1</v>
-      </c>
-      <c r="I72" s="2">
         <v>18</v>
       </c>
+      <c r="I72" s="2" t="s">
+        <v>77</v>
+      </c>
       <c r="J72" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="K72" s="2" t="s">
-        <v>77</v>
-      </c>
       <c r="L72" s="2">
         <v>1</v>
       </c>
-      <c r="M72" s="2"/>
+      <c r="M72" s="2">
+        <v>1</v>
+      </c>
       <c r="N72" s="2"/>
       <c r="O72" s="2"/>
-      <c r="P72" s="2">
-        <v>1</v>
-      </c>
-      <c r="Q72" s="2"/>
+      <c r="P72" s="2"/>
+      <c r="Q72" s="2">
+        <v>1</v>
+      </c>
       <c r="R72" s="2"/>
       <c r="S72" s="2"/>
       <c r="T72" s="2"/>
       <c r="U72" s="2"/>
       <c r="V72" s="2"/>
-    </row>
-    <row r="73" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W72" s="2"/>
+    </row>
+    <row r="73" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A73" s="2">
         <v>72</v>
       </c>
@@ -4881,24 +4906,23 @@
         <v>12</v>
       </c>
       <c r="H73" s="2">
-        <v>1</v>
-      </c>
-      <c r="I73" s="2">
         <v>7.4</v>
       </c>
+      <c r="I73" s="2" t="s">
+        <v>77</v>
+      </c>
       <c r="J73" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="K73" s="2" t="s">
-        <v>77</v>
-      </c>
       <c r="L73" s="2">
         <v>1</v>
       </c>
       <c r="M73" s="2">
         <v>1</v>
       </c>
-      <c r="N73" s="2"/>
+      <c r="N73" s="2">
+        <v>1</v>
+      </c>
       <c r="O73" s="2"/>
       <c r="P73" s="2"/>
       <c r="Q73" s="2"/>
@@ -4907,8 +4931,9 @@
       <c r="T73" s="2"/>
       <c r="U73" s="2"/>
       <c r="V73" s="2"/>
-    </row>
-    <row r="74" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W73" s="2"/>
+    </row>
+    <row r="74" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A74" s="2">
         <v>73</v>
       </c>
@@ -4931,24 +4956,23 @@
         <v>12</v>
       </c>
       <c r="H74" s="2">
-        <v>1</v>
-      </c>
-      <c r="I74" s="2">
         <v>4.2</v>
+      </c>
+      <c r="I74" s="2" t="s">
+        <v>25</v>
       </c>
       <c r="J74" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="K74" s="2" t="s">
-        <v>25</v>
-      </c>
       <c r="L74" s="2">
         <v>1</v>
       </c>
       <c r="M74" s="2">
         <v>1</v>
       </c>
-      <c r="N74" s="2"/>
+      <c r="N74" s="2">
+        <v>1</v>
+      </c>
       <c r="O74" s="2"/>
       <c r="P74" s="2"/>
       <c r="Q74" s="2"/>
@@ -4957,8 +4981,9 @@
       <c r="T74" s="2"/>
       <c r="U74" s="2"/>
       <c r="V74" s="2"/>
-    </row>
-    <row r="75" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W74" s="2"/>
+    </row>
+    <row r="75" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A75" s="2">
         <v>74</v>
       </c>
@@ -4981,22 +5006,21 @@
         <v>12</v>
       </c>
       <c r="H75" s="2">
-        <v>1</v>
-      </c>
-      <c r="I75" s="2">
         <v>7</v>
       </c>
+      <c r="I75" s="2"/>
       <c r="J75" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="K75" s="2"/>
       <c r="L75" s="2">
         <v>1</v>
       </c>
       <c r="M75" s="2">
         <v>1</v>
       </c>
-      <c r="N75" s="2"/>
+      <c r="N75" s="2">
+        <v>1</v>
+      </c>
       <c r="O75" s="2"/>
       <c r="P75" s="2"/>
       <c r="Q75" s="2"/>
@@ -5005,8 +5029,9 @@
       <c r="T75" s="2"/>
       <c r="U75" s="2"/>
       <c r="V75" s="2"/>
-    </row>
-    <row r="76" spans="1:22" ht="30" x14ac:dyDescent="0.25">
+      <c r="W75" s="2"/>
+    </row>
+    <row r="76" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="A76" s="2">
         <v>75</v>
       </c>
@@ -5029,24 +5054,23 @@
         <v>61</v>
       </c>
       <c r="H76" s="2">
-        <v>1</v>
-      </c>
-      <c r="I76" s="2">
         <v>6.6</v>
       </c>
+      <c r="I76" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="J76" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="K76" s="2" t="s">
-        <v>25</v>
-      </c>
       <c r="L76" s="2">
         <v>1</v>
       </c>
       <c r="M76" s="2">
         <v>1</v>
       </c>
-      <c r="N76" s="2"/>
+      <c r="N76" s="2">
+        <v>1</v>
+      </c>
       <c r="O76" s="2"/>
       <c r="P76" s="2"/>
       <c r="Q76" s="2"/>
@@ -5055,8 +5079,9 @@
       <c r="T76" s="2"/>
       <c r="U76" s="2"/>
       <c r="V76" s="2"/>
-    </row>
-    <row r="77" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W76" s="2"/>
+    </row>
+    <row r="77" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A77" s="2">
         <v>76</v>
       </c>
@@ -5079,24 +5104,23 @@
         <v>12</v>
       </c>
       <c r="H77" s="2">
-        <v>1</v>
-      </c>
-      <c r="I77" s="2">
         <v>6</v>
       </c>
+      <c r="I77" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="J77" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="K77" s="2" t="s">
-        <v>25</v>
-      </c>
       <c r="L77" s="2">
         <v>1</v>
       </c>
       <c r="M77" s="2">
         <v>1</v>
       </c>
-      <c r="N77" s="2"/>
+      <c r="N77" s="2">
+        <v>1</v>
+      </c>
       <c r="O77" s="2"/>
       <c r="P77" s="2"/>
       <c r="Q77" s="2"/>
@@ -5105,8 +5129,9 @@
       <c r="T77" s="2"/>
       <c r="U77" s="2"/>
       <c r="V77" s="2"/>
-    </row>
-    <row r="78" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W77" s="2"/>
+    </row>
+    <row r="78" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A78" s="2">
         <v>77</v>
       </c>
@@ -5129,24 +5154,23 @@
         <v>12</v>
       </c>
       <c r="H78" s="2">
-        <v>1</v>
-      </c>
-      <c r="I78" s="2">
         <v>3</v>
       </c>
+      <c r="I78" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="J78" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="K78" s="2" t="s">
-        <v>28</v>
-      </c>
       <c r="L78" s="2">
         <v>1</v>
       </c>
       <c r="M78" s="2">
         <v>1</v>
       </c>
-      <c r="N78" s="2"/>
+      <c r="N78" s="2">
+        <v>1</v>
+      </c>
       <c r="O78" s="2"/>
       <c r="P78" s="2"/>
       <c r="Q78" s="2"/>
@@ -5155,8 +5179,9 @@
       <c r="T78" s="2"/>
       <c r="U78" s="2"/>
       <c r="V78" s="2"/>
-    </row>
-    <row r="79" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W78" s="2"/>
+    </row>
+    <row r="79" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A79" s="2">
         <v>78</v>
       </c>
@@ -5179,24 +5204,23 @@
         <v>12</v>
       </c>
       <c r="H79" s="2">
-        <v>2</v>
-      </c>
-      <c r="I79" s="2">
         <v>6</v>
       </c>
+      <c r="I79" s="2" t="s">
+        <v>238</v>
+      </c>
       <c r="J79" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="K79" s="2" t="s">
-        <v>238</v>
-      </c>
       <c r="L79" s="2">
         <v>2</v>
       </c>
       <c r="M79" s="2">
         <v>2</v>
       </c>
-      <c r="N79" s="2"/>
+      <c r="N79" s="2">
+        <v>2</v>
+      </c>
       <c r="O79" s="2"/>
       <c r="P79" s="2"/>
       <c r="Q79" s="2"/>
@@ -5205,8 +5229,9 @@
       <c r="T79" s="2"/>
       <c r="U79" s="2"/>
       <c r="V79" s="2"/>
-    </row>
-    <row r="80" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W79" s="2"/>
+    </row>
+    <row r="80" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A80" s="2">
         <v>79</v>
       </c>
@@ -5229,34 +5254,34 @@
         <v>42</v>
       </c>
       <c r="H80" s="2">
-        <v>1</v>
-      </c>
-      <c r="I80" s="2">
         <v>22</v>
       </c>
+      <c r="I80" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="J80" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="K80" s="2" t="s">
-        <v>28</v>
-      </c>
       <c r="L80" s="2">
         <v>1</v>
       </c>
-      <c r="M80" s="2"/>
+      <c r="M80" s="2">
+        <v>1</v>
+      </c>
       <c r="N80" s="2"/>
       <c r="O80" s="2"/>
-      <c r="P80" s="2">
-        <v>1</v>
-      </c>
-      <c r="Q80" s="2"/>
+      <c r="P80" s="2"/>
+      <c r="Q80" s="2">
+        <v>1</v>
+      </c>
       <c r="R80" s="2"/>
       <c r="S80" s="2"/>
       <c r="T80" s="2"/>
       <c r="U80" s="2"/>
       <c r="V80" s="2"/>
-    </row>
-    <row r="81" spans="1:22" ht="30" x14ac:dyDescent="0.25">
+      <c r="W80" s="2"/>
+    </row>
+    <row r="81" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="A81" s="2">
         <v>80</v>
       </c>
@@ -5279,38 +5304,38 @@
         <v>242</v>
       </c>
       <c r="H81" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="I81" s="2"/>
+      <c r="J81" s="2"/>
+      <c r="L81" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="I81" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="J81" s="2"/>
-      <c r="K81" s="2"/>
-      <c r="L81" s="7">
+      <c r="M81" s="7">
         <v>6</v>
       </c>
-      <c r="M81" s="2">
-        <v>2</v>
-      </c>
       <c r="N81" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O81" s="2">
         <v>1</v>
       </c>
-      <c r="P81" s="2"/>
-      <c r="Q81" s="2">
-        <v>1</v>
-      </c>
-      <c r="R81" s="2"/>
+      <c r="P81" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q81" s="2"/>
+      <c r="R81" s="2">
+        <v>1</v>
+      </c>
       <c r="S81" s="2"/>
-      <c r="T81" s="2">
-        <v>1</v>
-      </c>
-      <c r="U81" s="2"/>
+      <c r="T81" s="2"/>
+      <c r="U81" s="2">
+        <v>1</v>
+      </c>
       <c r="V81" s="2"/>
-    </row>
-    <row r="82" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W81" s="2"/>
+    </row>
+    <row r="82" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A82" s="2"/>
       <c r="B82" s="2"/>
       <c r="C82" s="2"/>
@@ -5319,57 +5344,57 @@
       <c r="F82" s="2"/>
       <c r="G82" s="2"/>
       <c r="H82" s="2"/>
-      <c r="I82" s="2"/>
+      <c r="I82" s="12" t="s">
+        <v>248</v>
+      </c>
       <c r="J82" s="2"/>
-      <c r="K82" s="10" t="s">
-        <v>248</v>
-      </c>
-      <c r="L82" s="11">
-        <f>SUM(L2:L81)</f>
+      <c r="L82" s="2"/>
+      <c r="M82" s="10">
+        <f t="shared" ref="M82:T82" si="0">SUM(M2:M81)</f>
         <v>162</v>
       </c>
-      <c r="M82" s="11">
-        <f>SUM(M2:M81)</f>
+      <c r="N82" s="10">
+        <f t="shared" si="0"/>
         <v>69</v>
       </c>
-      <c r="N82" s="11">
-        <f>SUM(N2:N81)</f>
+      <c r="O82" s="10">
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="O82" s="11">
-        <f>SUM(O2:O81)</f>
+      <c r="P82" s="10">
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="P82" s="11">
-        <f>SUM(P2:P81)</f>
+      <c r="Q82" s="10">
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="Q82" s="11">
-        <f>SUM(Q2:Q81)</f>
+      <c r="R82" s="10">
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="R82" s="11">
-        <f>SUM(R2:R81)</f>
+      <c r="S82" s="10">
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="S82" s="11">
-        <f>SUM(S2:S81)</f>
+      <c r="T82" s="10">
+        <f t="shared" si="0"/>
         <v>43</v>
       </c>
-      <c r="T82" s="11">
-        <f t="shared" ref="N82:V82" si="0">SUM(T2:T81)</f>
+      <c r="U82" s="10">
+        <f t="shared" ref="U82:W82" si="1">SUM(U2:U81)</f>
         <v>4</v>
       </c>
-      <c r="U82" s="11">
-        <f t="shared" si="0"/>
+      <c r="V82" s="10">
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="V82" s="11">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="83" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W82" s="10">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A83" s="2"/>
       <c r="B83" s="2"/>
       <c r="C83" s="2"/>
@@ -5378,37 +5403,37 @@
       <c r="F83" s="2"/>
       <c r="G83" s="2"/>
       <c r="H83" s="2"/>
-      <c r="I83" s="2"/>
+      <c r="I83" s="12"/>
       <c r="J83" s="2"/>
-      <c r="K83" s="10"/>
-      <c r="L83" s="12"/>
-      <c r="M83" s="12"/>
-      <c r="N83" s="12"/>
-      <c r="O83" s="12"/>
-      <c r="P83" s="12"/>
-      <c r="Q83" s="12"/>
-      <c r="R83" s="12"/>
-      <c r="S83" s="12"/>
-      <c r="T83" s="12"/>
-      <c r="U83" s="12"/>
-      <c r="V83" s="12"/>
+      <c r="L83" s="2"/>
+      <c r="M83" s="11"/>
+      <c r="N83" s="11"/>
+      <c r="O83" s="11"/>
+      <c r="P83" s="11"/>
+      <c r="Q83" s="11"/>
+      <c r="R83" s="11"/>
+      <c r="S83" s="11"/>
+      <c r="T83" s="11"/>
+      <c r="U83" s="11"/>
+      <c r="V83" s="11"/>
+      <c r="W83" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="W82:W83"/>
+    <mergeCell ref="I82:I83"/>
+    <mergeCell ref="M82:M83"/>
+    <mergeCell ref="N82:N83"/>
+    <mergeCell ref="O82:O83"/>
+    <mergeCell ref="P82:P83"/>
     <mergeCell ref="Q82:Q83"/>
     <mergeCell ref="R82:R83"/>
     <mergeCell ref="S82:S83"/>
     <mergeCell ref="T82:T83"/>
     <mergeCell ref="U82:U83"/>
     <mergeCell ref="V82:V83"/>
-    <mergeCell ref="K82:K83"/>
-    <mergeCell ref="L82:L83"/>
-    <mergeCell ref="M82:M83"/>
-    <mergeCell ref="N82:N83"/>
-    <mergeCell ref="O82:O83"/>
-    <mergeCell ref="P82:P83"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>